<commit_message>
grasshopper and locust attacking done
</commit_message>
<xml_diff>
--- a/characters info ORIGINAL JULY 2015.xlsx
+++ b/characters info ORIGINAL JULY 2015.xlsx
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1876,29 +1876,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G51" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I51" s="1" t="s">
+      <c r="H51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I51" s="4" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1980,29 +1980,29 @@
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F55" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G55" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H55" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I55" s="3" t="s">
+      <c r="I55" s="4" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>